<commit_message>
Added an blinking Heart after the kiss
</commit_message>
<xml_diff>
--- a/Software/Animation.xlsx
+++ b/Software/Animation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eduard/Git/PlantBuddy/Software/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esc/Git/PlantBuddy/Software/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF83AE0-5BE8-BF4E-AFBF-4645B1D2ADCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400E83E9-DBF2-D448-B72B-C0883076AEF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5020" windowWidth="28040" windowHeight="17360" xr2:uid="{EF37F636-A34D-9A4C-85A7-3D0E4513D72B}"/>
+    <workbookView xWindow="21860" yWindow="860" windowWidth="14140" windowHeight="22520" xr2:uid="{EF37F636-A34D-9A4C-85A7-3D0E4513D72B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Eyes</t>
   </si>
@@ -59,6 +59,12 @@
   <si>
     <t>center_smal</t>
   </si>
+  <si>
+    <t>Heart Large</t>
+  </si>
+  <si>
+    <t>Heart smal</t>
+  </si>
 </sst>
 </file>
 
@@ -73,7 +79,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -89,6 +95,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -185,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -202,6 +214,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -516,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28B7383B-3F2C-C84C-B31B-6ED1EF4A681D}">
-  <dimension ref="A1:J80"/>
+  <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="200" workbookViewId="0">
+      <selection activeCell="J99" sqref="J99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1117,6 +1133,184 @@
       <c r="G80" s="8"/>
       <c r="H80" s="9"/>
     </row>
+    <row r="85" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A86" s="1"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
+      <c r="H86" s="3"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A87" s="4"/>
+      <c r="B87" s="17"/>
+      <c r="C87" s="17"/>
+      <c r="D87" s="5"/>
+      <c r="E87" s="5"/>
+      <c r="F87" s="17"/>
+      <c r="G87" s="17"/>
+      <c r="H87" s="6"/>
+      <c r="J87" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A88" s="16"/>
+      <c r="B88" s="17"/>
+      <c r="C88" s="17"/>
+      <c r="D88" s="17"/>
+      <c r="E88" s="17"/>
+      <c r="F88" s="17"/>
+      <c r="G88" s="17"/>
+      <c r="H88" s="18"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A89" s="16"/>
+      <c r="B89" s="17"/>
+      <c r="C89" s="17"/>
+      <c r="D89" s="17"/>
+      <c r="E89" s="17"/>
+      <c r="F89" s="17"/>
+      <c r="G89" s="17"/>
+      <c r="H89" s="18"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A90" s="16"/>
+      <c r="B90" s="17"/>
+      <c r="C90" s="17"/>
+      <c r="D90" s="17"/>
+      <c r="E90" s="17"/>
+      <c r="F90" s="17"/>
+      <c r="G90" s="17"/>
+      <c r="H90" s="18"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A91" s="4"/>
+      <c r="B91" s="17"/>
+      <c r="C91" s="17"/>
+      <c r="D91" s="17"/>
+      <c r="E91" s="17"/>
+      <c r="F91" s="17"/>
+      <c r="G91" s="17"/>
+      <c r="H91" s="6"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A92" s="4"/>
+      <c r="B92" s="5"/>
+      <c r="C92" s="17"/>
+      <c r="D92" s="17"/>
+      <c r="E92" s="17"/>
+      <c r="F92" s="17"/>
+      <c r="G92" s="5"/>
+      <c r="H92" s="6"/>
+    </row>
+    <row r="93" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="7"/>
+      <c r="B93" s="8"/>
+      <c r="C93" s="8"/>
+      <c r="D93" s="19"/>
+      <c r="E93" s="19"/>
+      <c r="F93" s="8"/>
+      <c r="G93" s="8"/>
+      <c r="H93" s="9"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A94" s="5"/>
+      <c r="B94" s="5"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="5"/>
+      <c r="G94" s="5"/>
+      <c r="H94" s="5"/>
+    </row>
+    <row r="95" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A96" s="1"/>
+      <c r="B96" s="2"/>
+      <c r="C96" s="2"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+      <c r="G96" s="2"/>
+      <c r="H96" s="3"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A97" s="4"/>
+      <c r="B97" s="5"/>
+      <c r="C97" s="5"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="5"/>
+      <c r="F97" s="5"/>
+      <c r="G97" s="5"/>
+      <c r="H97" s="6"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A98" s="4"/>
+      <c r="B98" s="5"/>
+      <c r="C98" s="17"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="17"/>
+      <c r="F98" s="5"/>
+      <c r="G98" s="5"/>
+      <c r="H98" s="6"/>
+      <c r="J98" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A99" s="4"/>
+      <c r="B99" s="17"/>
+      <c r="C99" s="17"/>
+      <c r="D99" s="17"/>
+      <c r="E99" s="17"/>
+      <c r="F99" s="17"/>
+      <c r="G99" s="5"/>
+      <c r="H99" s="6"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A100" s="4"/>
+      <c r="B100" s="17"/>
+      <c r="C100" s="17"/>
+      <c r="D100" s="17"/>
+      <c r="E100" s="17"/>
+      <c r="F100" s="17"/>
+      <c r="G100" s="5"/>
+      <c r="H100" s="6"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A101" s="4"/>
+      <c r="B101" s="5"/>
+      <c r="C101" s="17"/>
+      <c r="D101" s="17"/>
+      <c r="E101" s="17"/>
+      <c r="F101" s="5"/>
+      <c r="G101" s="5"/>
+      <c r="H101" s="6"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A102" s="4"/>
+      <c r="B102" s="5"/>
+      <c r="C102" s="5"/>
+      <c r="D102" s="17"/>
+      <c r="E102" s="5"/>
+      <c r="F102" s="5"/>
+      <c r="G102" s="5"/>
+      <c r="H102" s="6"/>
+    </row>
+    <row r="103" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="7"/>
+      <c r="B103" s="8"/>
+      <c r="C103" s="8"/>
+      <c r="D103" s="8"/>
+      <c r="E103" s="8"/>
+      <c r="F103" s="8"/>
+      <c r="G103" s="8"/>
+      <c r="H103" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated readme and Animation
</commit_message>
<xml_diff>
--- a/Software/Animation.xlsx
+++ b/Software/Animation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esc/Git/PlantBuddy/Software/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400E83E9-DBF2-D448-B72B-C0883076AEF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B87B25-89B3-C149-BE01-0FA95A6290A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21860" yWindow="860" windowWidth="14140" windowHeight="22520" xr2:uid="{EF37F636-A34D-9A4C-85A7-3D0E4513D72B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{EF37F636-A34D-9A4C-85A7-3D0E4513D72B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Eyes</t>
   </si>
@@ -65,6 +65,9 @@
   <si>
     <t>Heart smal</t>
   </si>
+  <si>
+    <t>BLINK TONG OUT</t>
+  </si>
 </sst>
 </file>
 
@@ -79,7 +82,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -101,6 +104,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -197,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -218,6 +233,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -532,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28B7383B-3F2C-C84C-B31B-6ED1EF4A681D}">
-  <dimension ref="A1:J103"/>
+  <dimension ref="A1:J153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="200" workbookViewId="0">
-      <selection activeCell="J99" sqref="J99"/>
+    <sheetView tabSelected="1" topLeftCell="A138" zoomScale="200" workbookViewId="0">
+      <selection activeCell="L162" sqref="L162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1311,6 +1332,414 @@
       <c r="G103" s="8"/>
       <c r="H103" s="9"/>
     </row>
+    <row r="105" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A106" s="1"/>
+      <c r="B106" s="2"/>
+      <c r="C106" s="2"/>
+      <c r="D106" s="2"/>
+      <c r="E106" s="2"/>
+      <c r="F106" s="2"/>
+      <c r="G106" s="2"/>
+      <c r="H106" s="3"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A107" s="4"/>
+      <c r="B107" s="20"/>
+      <c r="C107" s="20"/>
+      <c r="D107" s="5"/>
+      <c r="E107" s="5"/>
+      <c r="F107" s="11"/>
+      <c r="G107" s="11"/>
+      <c r="H107" s="6"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A108" s="4"/>
+      <c r="B108" s="20"/>
+      <c r="C108" s="20"/>
+      <c r="D108" s="5"/>
+      <c r="E108" s="5"/>
+      <c r="F108" s="20"/>
+      <c r="G108" s="20"/>
+      <c r="H108" s="6"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A109" s="4"/>
+      <c r="B109" s="5"/>
+      <c r="C109" s="5"/>
+      <c r="D109" s="5"/>
+      <c r="E109" s="5"/>
+      <c r="F109" s="5"/>
+      <c r="G109" s="5"/>
+      <c r="H109" s="6"/>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A110" s="4"/>
+      <c r="B110" s="5"/>
+      <c r="C110" s="5"/>
+      <c r="D110" s="5"/>
+      <c r="E110" s="21"/>
+      <c r="F110" s="11"/>
+      <c r="G110" s="21"/>
+      <c r="H110" s="6"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A111" s="4"/>
+      <c r="B111" s="5"/>
+      <c r="C111" s="5"/>
+      <c r="D111" s="5"/>
+      <c r="E111" s="5"/>
+      <c r="F111" s="21"/>
+      <c r="G111" s="5"/>
+      <c r="H111" s="6"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A112" s="4"/>
+      <c r="B112" s="5"/>
+      <c r="C112" s="5"/>
+      <c r="D112" s="5"/>
+      <c r="E112" s="21"/>
+      <c r="F112" s="5"/>
+      <c r="G112" s="21"/>
+      <c r="H112" s="6"/>
+    </row>
+    <row r="113" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="7"/>
+      <c r="B113" s="8"/>
+      <c r="C113" s="8"/>
+      <c r="D113" s="8"/>
+      <c r="E113" s="8"/>
+      <c r="F113" s="8"/>
+      <c r="G113" s="8"/>
+      <c r="H113" s="9"/>
+    </row>
+    <row r="115" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A116" s="1"/>
+      <c r="B116" s="2"/>
+      <c r="C116" s="2"/>
+      <c r="D116" s="2"/>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2"/>
+      <c r="G116" s="2"/>
+      <c r="H116" s="3"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A117" s="4"/>
+      <c r="B117" s="11"/>
+      <c r="C117" s="11"/>
+      <c r="D117" s="5"/>
+      <c r="E117" s="5"/>
+      <c r="F117" s="11"/>
+      <c r="G117" s="11"/>
+      <c r="H117" s="6"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A118" s="4"/>
+      <c r="B118" s="20"/>
+      <c r="C118" s="20"/>
+      <c r="D118" s="5"/>
+      <c r="E118" s="5"/>
+      <c r="F118" s="20"/>
+      <c r="G118" s="20"/>
+      <c r="H118" s="6"/>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A119" s="4"/>
+      <c r="B119" s="5"/>
+      <c r="C119" s="5"/>
+      <c r="D119" s="5"/>
+      <c r="E119" s="5"/>
+      <c r="F119" s="5"/>
+      <c r="G119" s="5"/>
+      <c r="H119" s="6"/>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A120" s="4"/>
+      <c r="B120" s="11"/>
+      <c r="C120" s="20"/>
+      <c r="D120" s="20"/>
+      <c r="E120" s="20"/>
+      <c r="F120" s="20"/>
+      <c r="G120" s="11"/>
+      <c r="H120" s="24"/>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A121" s="23"/>
+      <c r="B121" s="20"/>
+      <c r="C121" s="11"/>
+      <c r="D121" s="11"/>
+      <c r="E121" s="11"/>
+      <c r="F121" s="11"/>
+      <c r="G121" s="20"/>
+      <c r="H121" s="24"/>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A122" s="4"/>
+      <c r="B122" s="11"/>
+      <c r="C122" s="20"/>
+      <c r="D122" s="20"/>
+      <c r="E122" s="20"/>
+      <c r="F122" s="20"/>
+      <c r="G122" s="11"/>
+      <c r="H122" s="24"/>
+    </row>
+    <row r="123" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="7"/>
+      <c r="B123" s="22"/>
+      <c r="C123" s="22"/>
+      <c r="D123" s="22"/>
+      <c r="E123" s="22"/>
+      <c r="F123" s="22"/>
+      <c r="G123" s="22"/>
+      <c r="H123" s="25"/>
+    </row>
+    <row r="125" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A126" s="1"/>
+      <c r="B126" s="2"/>
+      <c r="C126" s="2"/>
+      <c r="D126" s="2"/>
+      <c r="E126" s="2"/>
+      <c r="F126" s="2"/>
+      <c r="G126" s="2"/>
+      <c r="H126" s="3"/>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A127" s="4"/>
+      <c r="B127" s="5"/>
+      <c r="C127" s="5"/>
+      <c r="D127" s="5"/>
+      <c r="E127" s="5"/>
+      <c r="F127" s="5"/>
+      <c r="G127" s="5"/>
+      <c r="H127" s="6"/>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A128" s="4"/>
+      <c r="B128" s="20"/>
+      <c r="C128" s="20"/>
+      <c r="D128" s="5"/>
+      <c r="E128" s="5"/>
+      <c r="F128" s="20"/>
+      <c r="G128" s="20"/>
+      <c r="H128" s="6"/>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A129" s="4"/>
+      <c r="B129" s="5"/>
+      <c r="C129" s="5"/>
+      <c r="D129" s="5"/>
+      <c r="E129" s="5"/>
+      <c r="F129" s="5"/>
+      <c r="G129" s="5"/>
+      <c r="H129" s="6"/>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A130" s="4"/>
+      <c r="B130" s="5"/>
+      <c r="C130" s="5"/>
+      <c r="D130" s="5"/>
+      <c r="E130" s="5"/>
+      <c r="F130" s="5"/>
+      <c r="G130" s="5"/>
+      <c r="H130" s="6"/>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A131" s="4"/>
+      <c r="B131" s="20"/>
+      <c r="C131" s="20"/>
+      <c r="D131" s="20"/>
+      <c r="E131" s="20"/>
+      <c r="F131" s="20"/>
+      <c r="G131" s="20"/>
+      <c r="H131" s="6"/>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A132" s="4"/>
+      <c r="B132" s="5"/>
+      <c r="C132" s="5"/>
+      <c r="D132" s="5"/>
+      <c r="E132" s="5"/>
+      <c r="F132" s="5"/>
+      <c r="G132" s="5"/>
+      <c r="H132" s="6"/>
+    </row>
+    <row r="133" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="7"/>
+      <c r="B133" s="8"/>
+      <c r="C133" s="8"/>
+      <c r="D133" s="8"/>
+      <c r="E133" s="8"/>
+      <c r="F133" s="8"/>
+      <c r="G133" s="8"/>
+      <c r="H133" s="9"/>
+    </row>
+    <row r="135" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A136" s="1"/>
+      <c r="B136" s="2"/>
+      <c r="C136" s="2"/>
+      <c r="D136" s="2"/>
+      <c r="E136" s="2"/>
+      <c r="F136" s="2"/>
+      <c r="G136" s="2"/>
+      <c r="H136" s="3"/>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A137" s="4"/>
+      <c r="B137" s="20"/>
+      <c r="C137" s="20"/>
+      <c r="D137" s="5"/>
+      <c r="E137" s="5"/>
+      <c r="F137" s="20"/>
+      <c r="G137" s="20"/>
+      <c r="H137" s="6"/>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A138" s="4"/>
+      <c r="B138" s="20"/>
+      <c r="C138" s="20"/>
+      <c r="D138" s="5"/>
+      <c r="E138" s="5"/>
+      <c r="F138" s="20"/>
+      <c r="G138" s="20"/>
+      <c r="H138" s="6"/>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A139" s="4"/>
+      <c r="B139" s="5"/>
+      <c r="C139" s="5"/>
+      <c r="D139" s="5"/>
+      <c r="E139" s="5"/>
+      <c r="F139" s="5"/>
+      <c r="G139" s="5"/>
+      <c r="H139" s="6"/>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A140" s="4"/>
+      <c r="B140" s="5"/>
+      <c r="C140" s="5"/>
+      <c r="D140" s="5"/>
+      <c r="E140" s="5"/>
+      <c r="F140" s="5"/>
+      <c r="G140" s="5"/>
+      <c r="H140" s="6"/>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A141" s="4"/>
+      <c r="B141" s="20"/>
+      <c r="C141" s="20"/>
+      <c r="D141" s="20"/>
+      <c r="E141" s="20"/>
+      <c r="F141" s="20"/>
+      <c r="G141" s="20"/>
+      <c r="H141" s="6"/>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A142" s="4"/>
+      <c r="B142" s="5"/>
+      <c r="C142" s="5"/>
+      <c r="D142" s="5"/>
+      <c r="E142" s="5"/>
+      <c r="F142" s="5"/>
+      <c r="G142" s="5"/>
+      <c r="H142" s="6"/>
+    </row>
+    <row r="143" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="7"/>
+      <c r="B143" s="8"/>
+      <c r="C143" s="8"/>
+      <c r="D143" s="8"/>
+      <c r="E143" s="8"/>
+      <c r="F143" s="8"/>
+      <c r="G143" s="8"/>
+      <c r="H143" s="9"/>
+    </row>
+    <row r="145" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A146" s="1"/>
+      <c r="B146" s="2"/>
+      <c r="C146" s="2"/>
+      <c r="D146" s="2"/>
+      <c r="E146" s="2"/>
+      <c r="F146" s="2"/>
+      <c r="G146" s="2"/>
+      <c r="H146" s="3"/>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A147" s="4"/>
+      <c r="B147" s="20"/>
+      <c r="C147" s="20"/>
+      <c r="D147" s="5"/>
+      <c r="E147" s="5"/>
+      <c r="F147" s="5"/>
+      <c r="G147" s="5"/>
+      <c r="H147" s="6"/>
+      <c r="J147" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A148" s="4"/>
+      <c r="B148" s="14"/>
+      <c r="C148" s="14"/>
+      <c r="D148" s="5"/>
+      <c r="E148" s="5"/>
+      <c r="F148" s="14"/>
+      <c r="G148" s="14"/>
+      <c r="H148" s="6"/>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A149" s="4"/>
+      <c r="B149" s="5"/>
+      <c r="C149" s="5"/>
+      <c r="D149" s="5"/>
+      <c r="E149" s="5"/>
+      <c r="F149" s="5"/>
+      <c r="G149" s="5"/>
+      <c r="H149" s="6"/>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A150" s="4"/>
+      <c r="B150" s="5"/>
+      <c r="C150" s="5"/>
+      <c r="D150" s="5"/>
+      <c r="E150" s="5"/>
+      <c r="F150" s="5"/>
+      <c r="G150" s="5"/>
+      <c r="H150" s="6"/>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A151" s="4"/>
+      <c r="B151" s="14"/>
+      <c r="C151" s="5"/>
+      <c r="D151" s="5"/>
+      <c r="E151" s="5"/>
+      <c r="F151" s="5"/>
+      <c r="G151" s="14"/>
+      <c r="H151" s="6"/>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A152" s="4"/>
+      <c r="B152" s="5"/>
+      <c r="C152" s="14"/>
+      <c r="D152" s="14"/>
+      <c r="E152" s="17"/>
+      <c r="F152" s="17"/>
+      <c r="G152" s="5"/>
+      <c r="H152" s="6"/>
+    </row>
+    <row r="153" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="7"/>
+      <c r="B153" s="8"/>
+      <c r="C153" s="8"/>
+      <c r="D153" s="8"/>
+      <c r="E153" s="19"/>
+      <c r="F153" s="19"/>
+      <c r="G153" s="8"/>
+      <c r="H153" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added animation for roling face
</commit_message>
<xml_diff>
--- a/Software/Animation.xlsx
+++ b/Software/Animation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esc/Git/PlantBuddy/Software/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B87B25-89B3-C149-BE01-0FA95A6290A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FA1756-8C26-E843-B1FB-406AC492AB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{EF37F636-A34D-9A4C-85A7-3D0E4513D72B}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="18840" windowHeight="22520" xr2:uid="{EF37F636-A34D-9A4C-85A7-3D0E4513D72B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -553,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28B7383B-3F2C-C84C-B31B-6ED1EF4A681D}">
-  <dimension ref="A1:J153"/>
+  <dimension ref="A1:J273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" zoomScale="200" workbookViewId="0">
-      <selection activeCell="L162" sqref="L162"/>
+    <sheetView tabSelected="1" topLeftCell="A248" zoomScale="200" workbookViewId="0">
+      <selection activeCell="L257" sqref="L257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1740,6 +1740,978 @@
       <c r="G153" s="8"/>
       <c r="H153" s="9"/>
     </row>
+    <row r="155" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A156" s="1"/>
+      <c r="B156" s="2"/>
+      <c r="C156" s="2"/>
+      <c r="D156" s="2"/>
+      <c r="E156" s="2"/>
+      <c r="F156" s="2"/>
+      <c r="G156" s="2"/>
+      <c r="H156" s="3"/>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A157" s="12"/>
+      <c r="B157" s="10"/>
+      <c r="C157" s="5"/>
+      <c r="D157" s="5"/>
+      <c r="E157" s="10"/>
+      <c r="F157" s="10"/>
+      <c r="G157" s="5"/>
+      <c r="H157" s="6"/>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A158" s="12"/>
+      <c r="B158" s="10"/>
+      <c r="C158" s="5"/>
+      <c r="D158" s="5"/>
+      <c r="E158" s="10"/>
+      <c r="F158" s="10"/>
+      <c r="G158" s="5"/>
+      <c r="H158" s="6"/>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A159" s="4"/>
+      <c r="B159" s="5"/>
+      <c r="C159" s="5"/>
+      <c r="D159" s="5"/>
+      <c r="E159" s="5"/>
+      <c r="F159" s="5"/>
+      <c r="G159" s="5"/>
+      <c r="H159" s="6"/>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A160" s="4"/>
+      <c r="B160" s="5"/>
+      <c r="C160" s="5"/>
+      <c r="D160" s="5"/>
+      <c r="E160" s="5"/>
+      <c r="F160" s="5"/>
+      <c r="G160" s="5"/>
+      <c r="H160" s="6"/>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A161" s="12"/>
+      <c r="B161" s="5"/>
+      <c r="C161" s="5"/>
+      <c r="D161" s="5"/>
+      <c r="E161" s="5"/>
+      <c r="F161" s="10"/>
+      <c r="G161" s="5"/>
+      <c r="H161" s="6"/>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A162" s="4"/>
+      <c r="B162" s="10"/>
+      <c r="C162" s="10"/>
+      <c r="D162" s="10"/>
+      <c r="E162" s="10"/>
+      <c r="F162" s="5"/>
+      <c r="G162" s="5"/>
+      <c r="H162" s="6"/>
+    </row>
+    <row r="163" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="7"/>
+      <c r="B163" s="8"/>
+      <c r="C163" s="8"/>
+      <c r="D163" s="8"/>
+      <c r="E163" s="8"/>
+      <c r="F163" s="8"/>
+      <c r="G163" s="8"/>
+      <c r="H163" s="9"/>
+    </row>
+    <row r="165" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A166" s="1"/>
+      <c r="B166" s="2"/>
+      <c r="C166" s="2"/>
+      <c r="D166" s="2"/>
+      <c r="E166" s="2"/>
+      <c r="F166" s="2"/>
+      <c r="G166" s="2"/>
+      <c r="H166" s="3"/>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A167" s="12"/>
+      <c r="B167" s="5"/>
+      <c r="C167" s="5"/>
+      <c r="D167" s="10"/>
+      <c r="E167" s="10"/>
+      <c r="F167" s="5"/>
+      <c r="G167" s="5"/>
+      <c r="H167" s="6"/>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A168" s="12"/>
+      <c r="B168" s="5"/>
+      <c r="C168" s="5"/>
+      <c r="D168" s="10"/>
+      <c r="E168" s="10"/>
+      <c r="F168" s="5"/>
+      <c r="G168" s="5"/>
+      <c r="H168" s="6"/>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A169" s="4"/>
+      <c r="B169" s="5"/>
+      <c r="C169" s="5"/>
+      <c r="D169" s="5"/>
+      <c r="E169" s="5"/>
+      <c r="F169" s="5"/>
+      <c r="G169" s="5"/>
+      <c r="H169" s="6"/>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A170" s="4"/>
+      <c r="B170" s="5"/>
+      <c r="C170" s="5"/>
+      <c r="D170" s="5"/>
+      <c r="E170" s="5"/>
+      <c r="F170" s="5"/>
+      <c r="G170" s="5"/>
+      <c r="H170" s="6"/>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A171" s="4"/>
+      <c r="B171" s="5"/>
+      <c r="C171" s="5"/>
+      <c r="D171" s="5"/>
+      <c r="E171" s="10"/>
+      <c r="F171" s="5"/>
+      <c r="G171" s="5"/>
+      <c r="H171" s="6"/>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A172" s="12"/>
+      <c r="B172" s="10"/>
+      <c r="C172" s="10"/>
+      <c r="D172" s="10"/>
+      <c r="E172" s="5"/>
+      <c r="F172" s="5"/>
+      <c r="G172" s="5"/>
+      <c r="H172" s="6"/>
+    </row>
+    <row r="173" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="7"/>
+      <c r="B173" s="8"/>
+      <c r="C173" s="8"/>
+      <c r="D173" s="8"/>
+      <c r="E173" s="8"/>
+      <c r="F173" s="8"/>
+      <c r="G173" s="8"/>
+      <c r="H173" s="9"/>
+    </row>
+    <row r="175" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A176" s="1"/>
+      <c r="B176" s="2"/>
+      <c r="C176" s="2"/>
+      <c r="D176" s="2"/>
+      <c r="E176" s="2"/>
+      <c r="F176" s="2"/>
+      <c r="G176" s="2"/>
+      <c r="H176" s="3"/>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A177" s="4"/>
+      <c r="B177" s="5"/>
+      <c r="C177" s="10"/>
+      <c r="D177" s="10"/>
+      <c r="E177" s="5"/>
+      <c r="F177" s="5"/>
+      <c r="G177" s="5"/>
+      <c r="H177" s="6"/>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A178" s="4"/>
+      <c r="B178" s="5"/>
+      <c r="C178" s="10"/>
+      <c r="D178" s="10"/>
+      <c r="E178" s="5"/>
+      <c r="F178" s="5"/>
+      <c r="G178" s="5"/>
+      <c r="H178" s="6"/>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A179" s="4"/>
+      <c r="B179" s="5"/>
+      <c r="C179" s="11"/>
+      <c r="D179" s="11"/>
+      <c r="E179" s="5"/>
+      <c r="F179" s="5"/>
+      <c r="G179" s="5"/>
+      <c r="H179" s="6"/>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A180" s="4"/>
+      <c r="B180" s="5"/>
+      <c r="C180" s="5"/>
+      <c r="D180" s="5"/>
+      <c r="E180" s="5"/>
+      <c r="F180" s="5"/>
+      <c r="G180" s="5"/>
+      <c r="H180" s="6"/>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A181" s="4"/>
+      <c r="B181" s="5"/>
+      <c r="C181" s="5"/>
+      <c r="D181" s="10"/>
+      <c r="E181" s="5"/>
+      <c r="F181" s="5"/>
+      <c r="G181" s="5"/>
+      <c r="H181" s="6"/>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A182" s="12"/>
+      <c r="B182" s="10"/>
+      <c r="C182" s="10"/>
+      <c r="D182" s="5"/>
+      <c r="E182" s="5"/>
+      <c r="F182" s="5"/>
+      <c r="G182" s="5"/>
+      <c r="H182" s="6"/>
+    </row>
+    <row r="183" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="7"/>
+      <c r="B183" s="8"/>
+      <c r="C183" s="8"/>
+      <c r="D183" s="8"/>
+      <c r="E183" s="8"/>
+      <c r="F183" s="8"/>
+      <c r="G183" s="8"/>
+      <c r="H183" s="9"/>
+    </row>
+    <row r="185" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A186" s="1"/>
+      <c r="B186" s="2"/>
+      <c r="C186" s="2"/>
+      <c r="D186" s="2"/>
+      <c r="E186" s="2"/>
+      <c r="F186" s="2"/>
+      <c r="G186" s="2"/>
+      <c r="H186" s="3"/>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A187" s="4"/>
+      <c r="B187" s="10"/>
+      <c r="C187" s="10"/>
+      <c r="D187" s="5"/>
+      <c r="E187" s="5"/>
+      <c r="F187" s="5"/>
+      <c r="G187" s="5"/>
+      <c r="H187" s="6"/>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A188" s="4"/>
+      <c r="B188" s="10"/>
+      <c r="C188" s="10"/>
+      <c r="D188" s="5"/>
+      <c r="E188" s="5"/>
+      <c r="F188" s="5"/>
+      <c r="G188" s="5"/>
+      <c r="H188" s="6"/>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A189" s="4"/>
+      <c r="B189" s="5"/>
+      <c r="C189" s="5"/>
+      <c r="D189" s="5"/>
+      <c r="E189" s="5"/>
+      <c r="F189" s="5"/>
+      <c r="G189" s="5"/>
+      <c r="H189" s="6"/>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A190" s="4"/>
+      <c r="B190" s="5"/>
+      <c r="C190" s="5"/>
+      <c r="D190" s="5"/>
+      <c r="E190" s="5"/>
+      <c r="F190" s="5"/>
+      <c r="G190" s="5"/>
+      <c r="H190" s="6"/>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A191" s="4"/>
+      <c r="B191" s="5"/>
+      <c r="C191" s="10"/>
+      <c r="D191" s="5"/>
+      <c r="E191" s="5"/>
+      <c r="F191" s="5"/>
+      <c r="G191" s="5"/>
+      <c r="H191" s="6"/>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A192" s="12"/>
+      <c r="B192" s="10"/>
+      <c r="C192" s="5"/>
+      <c r="D192" s="5"/>
+      <c r="E192" s="5"/>
+      <c r="F192" s="5"/>
+      <c r="G192" s="5"/>
+      <c r="H192" s="6"/>
+    </row>
+    <row r="193" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="7"/>
+      <c r="B193" s="8"/>
+      <c r="C193" s="8"/>
+      <c r="D193" s="8"/>
+      <c r="E193" s="8"/>
+      <c r="F193" s="8"/>
+      <c r="G193" s="8"/>
+      <c r="H193" s="9"/>
+    </row>
+    <row r="195" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A196" s="1"/>
+      <c r="B196" s="2"/>
+      <c r="C196" s="2"/>
+      <c r="D196" s="2"/>
+      <c r="E196" s="2"/>
+      <c r="F196" s="2"/>
+      <c r="G196" s="2"/>
+      <c r="H196" s="3"/>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A197" s="12"/>
+      <c r="B197" s="10"/>
+      <c r="C197" s="5"/>
+      <c r="D197" s="5"/>
+      <c r="E197" s="5"/>
+      <c r="F197" s="5"/>
+      <c r="G197" s="5"/>
+      <c r="H197" s="6"/>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A198" s="12"/>
+      <c r="B198" s="10"/>
+      <c r="C198" s="5"/>
+      <c r="D198" s="5"/>
+      <c r="E198" s="5"/>
+      <c r="F198" s="5"/>
+      <c r="G198" s="5"/>
+      <c r="H198" s="6"/>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A199" s="4"/>
+      <c r="B199" s="5"/>
+      <c r="C199" s="5"/>
+      <c r="D199" s="5"/>
+      <c r="E199" s="5"/>
+      <c r="F199" s="5"/>
+      <c r="G199" s="5"/>
+      <c r="H199" s="6"/>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A200" s="4"/>
+      <c r="B200" s="5"/>
+      <c r="C200" s="5"/>
+      <c r="D200" s="5"/>
+      <c r="E200" s="5"/>
+      <c r="F200" s="5"/>
+      <c r="G200" s="5"/>
+      <c r="H200" s="6"/>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A201" s="4"/>
+      <c r="B201" s="10"/>
+      <c r="C201" s="5"/>
+      <c r="D201" s="5"/>
+      <c r="E201" s="5"/>
+      <c r="F201" s="5"/>
+      <c r="G201" s="5"/>
+      <c r="H201" s="6"/>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A202" s="12"/>
+      <c r="B202" s="5"/>
+      <c r="C202" s="5"/>
+      <c r="D202" s="5"/>
+      <c r="E202" s="5"/>
+      <c r="F202" s="5"/>
+      <c r="G202" s="5"/>
+      <c r="H202" s="6"/>
+    </row>
+    <row r="203" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A203" s="7"/>
+      <c r="B203" s="8"/>
+      <c r="C203" s="8"/>
+      <c r="D203" s="8"/>
+      <c r="E203" s="8"/>
+      <c r="F203" s="8"/>
+      <c r="G203" s="8"/>
+      <c r="H203" s="9"/>
+    </row>
+    <row r="205" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A206" s="1"/>
+      <c r="B206" s="2"/>
+      <c r="C206" s="2"/>
+      <c r="D206" s="2"/>
+      <c r="E206" s="2"/>
+      <c r="F206" s="2"/>
+      <c r="G206" s="2"/>
+      <c r="H206" s="3"/>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A207" s="12"/>
+      <c r="B207" s="5"/>
+      <c r="C207" s="5"/>
+      <c r="D207" s="5"/>
+      <c r="E207" s="5"/>
+      <c r="F207" s="5"/>
+      <c r="G207" s="5"/>
+      <c r="H207" s="6"/>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A208" s="12"/>
+      <c r="B208" s="5"/>
+      <c r="C208" s="5"/>
+      <c r="D208" s="5"/>
+      <c r="E208" s="5"/>
+      <c r="F208" s="5"/>
+      <c r="G208" s="5"/>
+      <c r="H208" s="6"/>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A209" s="4"/>
+      <c r="B209" s="5"/>
+      <c r="C209" s="5"/>
+      <c r="D209" s="5"/>
+      <c r="E209" s="5"/>
+      <c r="F209" s="5"/>
+      <c r="G209" s="5"/>
+      <c r="H209" s="6"/>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A210" s="4"/>
+      <c r="B210" s="5"/>
+      <c r="C210" s="5"/>
+      <c r="D210" s="5"/>
+      <c r="E210" s="5"/>
+      <c r="F210" s="5"/>
+      <c r="G210" s="5"/>
+      <c r="H210" s="6"/>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A211" s="12"/>
+      <c r="B211" s="5"/>
+      <c r="C211" s="5"/>
+      <c r="D211" s="5"/>
+      <c r="E211" s="5"/>
+      <c r="F211" s="5"/>
+      <c r="G211" s="5"/>
+      <c r="H211" s="6"/>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A212" s="4"/>
+      <c r="B212" s="5"/>
+      <c r="C212" s="5"/>
+      <c r="D212" s="5"/>
+      <c r="E212" s="5"/>
+      <c r="F212" s="5"/>
+      <c r="G212" s="5"/>
+      <c r="H212" s="6"/>
+    </row>
+    <row r="213" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A213" s="7"/>
+      <c r="B213" s="8"/>
+      <c r="C213" s="8"/>
+      <c r="D213" s="8"/>
+      <c r="E213" s="8"/>
+      <c r="F213" s="8"/>
+      <c r="G213" s="8"/>
+      <c r="H213" s="9"/>
+    </row>
+    <row r="215" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A216" s="1"/>
+      <c r="B216" s="2"/>
+      <c r="C216" s="2"/>
+      <c r="D216" s="2"/>
+      <c r="E216" s="2"/>
+      <c r="F216" s="2"/>
+      <c r="G216" s="2"/>
+      <c r="H216" s="3"/>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A217" s="4"/>
+      <c r="B217" s="5"/>
+      <c r="C217" s="5"/>
+      <c r="D217" s="5"/>
+      <c r="E217" s="5"/>
+      <c r="F217" s="5"/>
+      <c r="G217" s="5"/>
+      <c r="H217" s="13"/>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A218" s="4"/>
+      <c r="B218" s="5"/>
+      <c r="C218" s="5"/>
+      <c r="D218" s="5"/>
+      <c r="E218" s="5"/>
+      <c r="F218" s="5"/>
+      <c r="G218" s="5"/>
+      <c r="H218" s="13"/>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A219" s="4"/>
+      <c r="B219" s="5"/>
+      <c r="C219" s="5"/>
+      <c r="D219" s="5"/>
+      <c r="E219" s="5"/>
+      <c r="F219" s="5"/>
+      <c r="G219" s="5"/>
+      <c r="H219" s="6"/>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A220" s="4"/>
+      <c r="B220" s="5"/>
+      <c r="C220" s="5"/>
+      <c r="D220" s="5"/>
+      <c r="E220" s="5"/>
+      <c r="F220" s="5"/>
+      <c r="G220" s="5"/>
+      <c r="H220" s="6"/>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A221" s="4"/>
+      <c r="B221" s="5"/>
+      <c r="C221" s="5"/>
+      <c r="D221" s="5"/>
+      <c r="E221" s="5"/>
+      <c r="F221" s="5"/>
+      <c r="G221" s="5"/>
+      <c r="H221" s="13"/>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A222" s="4"/>
+      <c r="B222" s="5"/>
+      <c r="C222" s="5"/>
+      <c r="D222" s="5"/>
+      <c r="E222" s="5"/>
+      <c r="F222" s="5"/>
+      <c r="G222" s="5"/>
+      <c r="H222" s="6"/>
+    </row>
+    <row r="223" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A223" s="7"/>
+      <c r="B223" s="8"/>
+      <c r="C223" s="8"/>
+      <c r="D223" s="8"/>
+      <c r="E223" s="8"/>
+      <c r="F223" s="8"/>
+      <c r="G223" s="8"/>
+      <c r="H223" s="9"/>
+    </row>
+    <row r="225" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A226" s="1"/>
+      <c r="B226" s="2"/>
+      <c r="C226" s="2"/>
+      <c r="D226" s="2"/>
+      <c r="E226" s="2"/>
+      <c r="F226" s="2"/>
+      <c r="G226" s="2"/>
+      <c r="H226" s="3"/>
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A227" s="4"/>
+      <c r="B227" s="5"/>
+      <c r="C227" s="5"/>
+      <c r="D227" s="5"/>
+      <c r="E227" s="5"/>
+      <c r="F227" s="5"/>
+      <c r="G227" s="10"/>
+      <c r="H227" s="13"/>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A228" s="4"/>
+      <c r="B228" s="5"/>
+      <c r="C228" s="5"/>
+      <c r="D228" s="5"/>
+      <c r="E228" s="5"/>
+      <c r="F228" s="5"/>
+      <c r="G228" s="10"/>
+      <c r="H228" s="13"/>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A229" s="4"/>
+      <c r="B229" s="5"/>
+      <c r="C229" s="5"/>
+      <c r="D229" s="5"/>
+      <c r="E229" s="5"/>
+      <c r="F229" s="5"/>
+      <c r="G229" s="5"/>
+      <c r="H229" s="6"/>
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A230" s="4"/>
+      <c r="B230" s="5"/>
+      <c r="C230" s="5"/>
+      <c r="D230" s="5"/>
+      <c r="E230" s="5"/>
+      <c r="F230" s="5"/>
+      <c r="G230" s="5"/>
+      <c r="H230" s="6"/>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A231" s="4"/>
+      <c r="B231" s="5"/>
+      <c r="C231" s="5"/>
+      <c r="D231" s="5"/>
+      <c r="E231" s="5"/>
+      <c r="F231" s="5"/>
+      <c r="G231" s="10"/>
+      <c r="H231" s="6"/>
+    </row>
+    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A232" s="4"/>
+      <c r="B232" s="5"/>
+      <c r="C232" s="5"/>
+      <c r="D232" s="5"/>
+      <c r="E232" s="5"/>
+      <c r="F232" s="5"/>
+      <c r="G232" s="5"/>
+      <c r="H232" s="13"/>
+    </row>
+    <row r="233" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A233" s="7"/>
+      <c r="B233" s="8"/>
+      <c r="C233" s="8"/>
+      <c r="D233" s="8"/>
+      <c r="E233" s="8"/>
+      <c r="F233" s="8"/>
+      <c r="G233" s="8"/>
+      <c r="H233" s="9"/>
+    </row>
+    <row r="235" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="236" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A236" s="1"/>
+      <c r="B236" s="2"/>
+      <c r="C236" s="2"/>
+      <c r="D236" s="2"/>
+      <c r="E236" s="2"/>
+      <c r="F236" s="2"/>
+      <c r="G236" s="2"/>
+      <c r="H236" s="3"/>
+    </row>
+    <row r="237" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A237" s="4"/>
+      <c r="B237" s="5"/>
+      <c r="C237" s="5"/>
+      <c r="D237" s="5"/>
+      <c r="E237" s="5"/>
+      <c r="F237" s="10"/>
+      <c r="G237" s="10"/>
+      <c r="H237" s="6"/>
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A238" s="4"/>
+      <c r="B238" s="5"/>
+      <c r="C238" s="5"/>
+      <c r="D238" s="5"/>
+      <c r="E238" s="5"/>
+      <c r="F238" s="10"/>
+      <c r="G238" s="10"/>
+      <c r="H238" s="6"/>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A239" s="4"/>
+      <c r="B239" s="5"/>
+      <c r="C239" s="5"/>
+      <c r="D239" s="5"/>
+      <c r="E239" s="5"/>
+      <c r="F239" s="5"/>
+      <c r="G239" s="5"/>
+      <c r="H239" s="6"/>
+    </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A240" s="4"/>
+      <c r="B240" s="5"/>
+      <c r="C240" s="5"/>
+      <c r="D240" s="5"/>
+      <c r="E240" s="5"/>
+      <c r="F240" s="5"/>
+      <c r="G240" s="5"/>
+      <c r="H240" s="6"/>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A241" s="4"/>
+      <c r="B241" s="5"/>
+      <c r="C241" s="5"/>
+      <c r="D241" s="5"/>
+      <c r="E241" s="5"/>
+      <c r="F241" s="10"/>
+      <c r="G241" s="5"/>
+      <c r="H241" s="6"/>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A242" s="4"/>
+      <c r="B242" s="5"/>
+      <c r="C242" s="5"/>
+      <c r="D242" s="5"/>
+      <c r="E242" s="5"/>
+      <c r="F242" s="5"/>
+      <c r="G242" s="10"/>
+      <c r="H242" s="13"/>
+    </row>
+    <row r="243" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A243" s="7"/>
+      <c r="B243" s="8"/>
+      <c r="C243" s="8"/>
+      <c r="D243" s="8"/>
+      <c r="E243" s="8"/>
+      <c r="F243" s="8"/>
+      <c r="G243" s="8"/>
+      <c r="H243" s="9"/>
+    </row>
+    <row r="245" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A246" s="1"/>
+      <c r="B246" s="2"/>
+      <c r="C246" s="2"/>
+      <c r="D246" s="2"/>
+      <c r="E246" s="2"/>
+      <c r="F246" s="2"/>
+      <c r="G246" s="2"/>
+      <c r="H246" s="3"/>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A247" s="4"/>
+      <c r="B247" s="5"/>
+      <c r="C247" s="5"/>
+      <c r="D247" s="5"/>
+      <c r="E247" s="10"/>
+      <c r="F247" s="10"/>
+      <c r="G247" s="5"/>
+      <c r="H247" s="6"/>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A248" s="4"/>
+      <c r="B248" s="5"/>
+      <c r="C248" s="5"/>
+      <c r="D248" s="5"/>
+      <c r="E248" s="10"/>
+      <c r="F248" s="10"/>
+      <c r="G248" s="5"/>
+      <c r="H248" s="6"/>
+    </row>
+    <row r="249" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A249" s="4"/>
+      <c r="B249" s="5"/>
+      <c r="C249" s="5"/>
+      <c r="D249" s="5"/>
+      <c r="E249" s="5"/>
+      <c r="F249" s="5"/>
+      <c r="G249" s="5"/>
+      <c r="H249" s="6"/>
+    </row>
+    <row r="250" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A250" s="4"/>
+      <c r="B250" s="5"/>
+      <c r="C250" s="5"/>
+      <c r="D250" s="5"/>
+      <c r="E250" s="5"/>
+      <c r="F250" s="5"/>
+      <c r="G250" s="5"/>
+      <c r="H250" s="6"/>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A251" s="4"/>
+      <c r="B251" s="5"/>
+      <c r="C251" s="5"/>
+      <c r="D251" s="5"/>
+      <c r="E251" s="10"/>
+      <c r="F251" s="5"/>
+      <c r="G251" s="5"/>
+      <c r="H251" s="6"/>
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A252" s="4"/>
+      <c r="B252" s="5"/>
+      <c r="C252" s="5"/>
+      <c r="D252" s="5"/>
+      <c r="E252" s="5"/>
+      <c r="F252" s="10"/>
+      <c r="G252" s="10"/>
+      <c r="H252" s="13"/>
+    </row>
+    <row r="253" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A253" s="7"/>
+      <c r="B253" s="8"/>
+      <c r="C253" s="8"/>
+      <c r="D253" s="8"/>
+      <c r="E253" s="8"/>
+      <c r="F253" s="8"/>
+      <c r="G253" s="8"/>
+      <c r="H253" s="9"/>
+    </row>
+    <row r="255" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="256" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A256" s="1"/>
+      <c r="B256" s="2"/>
+      <c r="C256" s="2"/>
+      <c r="D256" s="2"/>
+      <c r="E256" s="2"/>
+      <c r="F256" s="2"/>
+      <c r="G256" s="2"/>
+      <c r="H256" s="3"/>
+    </row>
+    <row r="257" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A257" s="4"/>
+      <c r="B257" s="5"/>
+      <c r="C257" s="5"/>
+      <c r="D257" s="10"/>
+      <c r="E257" s="10"/>
+      <c r="F257" s="5"/>
+      <c r="G257" s="5"/>
+      <c r="H257" s="13"/>
+    </row>
+    <row r="258" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A258" s="4"/>
+      <c r="B258" s="5"/>
+      <c r="C258" s="5"/>
+      <c r="D258" s="10"/>
+      <c r="E258" s="10"/>
+      <c r="F258" s="5"/>
+      <c r="G258" s="5"/>
+      <c r="H258" s="13"/>
+    </row>
+    <row r="259" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A259" s="4"/>
+      <c r="B259" s="5"/>
+      <c r="C259" s="5"/>
+      <c r="D259" s="5"/>
+      <c r="E259" s="5"/>
+      <c r="F259" s="5"/>
+      <c r="G259" s="5"/>
+      <c r="H259" s="6"/>
+    </row>
+    <row r="260" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A260" s="4"/>
+      <c r="B260" s="5"/>
+      <c r="C260" s="5"/>
+      <c r="D260" s="5"/>
+      <c r="E260" s="5"/>
+      <c r="F260" s="5"/>
+      <c r="G260" s="5"/>
+      <c r="H260" s="6"/>
+    </row>
+    <row r="261" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A261" s="4"/>
+      <c r="B261" s="5"/>
+      <c r="C261" s="5"/>
+      <c r="D261" s="10"/>
+      <c r="E261" s="5"/>
+      <c r="F261" s="5"/>
+      <c r="G261" s="5"/>
+      <c r="H261" s="6"/>
+    </row>
+    <row r="262" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A262" s="4"/>
+      <c r="B262" s="5"/>
+      <c r="C262" s="5"/>
+      <c r="D262" s="5"/>
+      <c r="E262" s="10"/>
+      <c r="F262" s="10"/>
+      <c r="G262" s="10"/>
+      <c r="H262" s="13"/>
+    </row>
+    <row r="263" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A263" s="7"/>
+      <c r="B263" s="8"/>
+      <c r="C263" s="8"/>
+      <c r="D263" s="8"/>
+      <c r="E263" s="8"/>
+      <c r="F263" s="8"/>
+      <c r="G263" s="8"/>
+      <c r="H263" s="9"/>
+    </row>
+    <row r="265" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="266" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A266" s="1"/>
+      <c r="B266" s="2"/>
+      <c r="C266" s="2"/>
+      <c r="D266" s="2"/>
+      <c r="E266" s="2"/>
+      <c r="F266" s="2"/>
+      <c r="G266" s="2"/>
+      <c r="H266" s="3"/>
+    </row>
+    <row r="267" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A267" s="4"/>
+      <c r="B267" s="5"/>
+      <c r="C267" s="10"/>
+      <c r="D267" s="10"/>
+      <c r="E267" s="5"/>
+      <c r="F267" s="5"/>
+      <c r="G267" s="10"/>
+      <c r="H267" s="13"/>
+    </row>
+    <row r="268" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A268" s="4"/>
+      <c r="B268" s="5"/>
+      <c r="C268" s="10"/>
+      <c r="D268" s="10"/>
+      <c r="E268" s="5"/>
+      <c r="F268" s="5"/>
+      <c r="G268" s="10"/>
+      <c r="H268" s="13"/>
+    </row>
+    <row r="269" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A269" s="4"/>
+      <c r="B269" s="5"/>
+      <c r="C269" s="5"/>
+      <c r="D269" s="5"/>
+      <c r="E269" s="5"/>
+      <c r="F269" s="5"/>
+      <c r="G269" s="5"/>
+      <c r="H269" s="6"/>
+    </row>
+    <row r="270" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A270" s="4"/>
+      <c r="B270" s="5"/>
+      <c r="C270" s="5"/>
+      <c r="D270" s="5"/>
+      <c r="E270" s="5"/>
+      <c r="F270" s="5"/>
+      <c r="G270" s="5"/>
+      <c r="H270" s="6"/>
+    </row>
+    <row r="271" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A271" s="4"/>
+      <c r="B271" s="5"/>
+      <c r="C271" s="10"/>
+      <c r="D271" s="5"/>
+      <c r="E271" s="5"/>
+      <c r="F271" s="5"/>
+      <c r="G271" s="5"/>
+      <c r="H271" s="13"/>
+    </row>
+    <row r="272" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A272" s="4"/>
+      <c r="B272" s="5"/>
+      <c r="C272" s="5"/>
+      <c r="D272" s="10"/>
+      <c r="E272" s="10"/>
+      <c r="F272" s="10"/>
+      <c r="G272" s="10"/>
+      <c r="H272" s="6"/>
+    </row>
+    <row r="273" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A273" s="7"/>
+      <c r="B273" s="8"/>
+      <c r="C273" s="8"/>
+      <c r="D273" s="8"/>
+      <c r="E273" s="8"/>
+      <c r="F273" s="8"/>
+      <c r="G273" s="8"/>
+      <c r="H273" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>